<commit_message>
Ability to import values for labels
</commit_message>
<xml_diff>
--- a/web/static/documents/fichier_exemple_ma_cantine.xlsx
+++ b/web/static/documents/fichier_exemple_ma_cantine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenfrancesroot/Develop/ma-cantine/web/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{58762451-41F3-E149-A606-AD196A06F0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6451EAEC-499B-2C4D-8E29-FF35CFFCE81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fichier_exemple_ma_cantine" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>SIRET</t>
   </si>
@@ -89,12 +89,21 @@
   </si>
   <si>
     <t>Secteur économique</t>
+  </si>
+  <si>
+    <t>Label Rouge</t>
+  </si>
+  <si>
+    <t>AOC / AOP / IGP</t>
+  </si>
+  <si>
+    <t>HVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -928,11 +937,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,9 +961,10 @@
     <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,8 +1010,17 @@
       <c r="O1" t="s">
         <v>20</v>
       </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1047,8 +1066,11 @@
       <c r="O2">
         <v>100</v>
       </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1093,6 +1115,9 @@
       </c>
       <c r="O3">
         <v>200</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend import update for simplified diagnostic
</commit_message>
<xml_diff>
--- a/web/static/documents/fichier_exemple_ma_cantine.xlsx
+++ b/web/static/documents/fichier_exemple_ma_cantine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenfrancesroot/Develop/ma-cantine/web/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6451EAEC-499B-2C4D-8E29-FF35CFFCE81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC8428B-579E-164D-96C7-C7B12F7E0D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>SIRET</t>
   </si>
@@ -82,22 +82,34 @@
     <t>Administration+Crèche</t>
   </si>
   <si>
-    <t>Qualité et durable (hors bio)</t>
-  </si>
-  <si>
     <t>Année du diagnostic</t>
   </si>
   <si>
     <t>Secteur économique</t>
   </si>
   <si>
-    <t>Label Rouge</t>
-  </si>
-  <si>
-    <t>AOC / AOP / IGP</t>
-  </si>
-  <si>
-    <t>HVE</t>
+    <t>SIQO</t>
+  </si>
+  <si>
+    <t>Environnement</t>
+  </si>
+  <si>
+    <t>Autre EGAlim</t>
+  </si>
+  <si>
+    <t>Viandes vollailes total</t>
+  </si>
+  <si>
+    <t>Viandes vollailles EGAlim</t>
+  </si>
+  <si>
+    <t>Viandes vollailles provenance France</t>
+  </si>
+  <si>
+    <t>Produits aquatiques total</t>
+  </si>
+  <si>
+    <t>Produits aquatiques EGAlim</t>
   </si>
 </sst>
 </file>
@@ -581,8 +593,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -938,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,67 +973,80 @@
     <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour des fichiers templates pour les imoprts massif
</commit_message>
<xml_diff>
--- a/web/static/documents/fichier_exemple_ma_cantine.xlsx
+++ b/web/static/documents/fichier_exemple_ma_cantine.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="fichier_exemple_ma_cantine" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="fichier_exemple_ma_cantine" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,73 +22,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
-    <t xml:space="preserve">SIRET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom de la cantine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code postal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIRET cuisine centrale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repas par jour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repas par an</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secteurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode de production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode de gestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secteur économique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestionnaires addtionnels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Année du diagnostic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environnement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autre EGAlim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailes total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailles EGAlim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailles provenance France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produits aquatiques total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produits aquatiques EGAlim</t>
+    <t xml:space="preserve">siret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_insee_commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_postal_commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_livreur_repas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_gestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">année_bilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_totale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_siqo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_environnemental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_autres_egalim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes_egalim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes_france</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_poissons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_poissons_egalim</t>
   </si>
   <si>
     <t xml:space="preserve">000 000 000 00000</t>
@@ -196,12 +196,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,253 +221,359 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="36.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="24.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="32.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="24.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>69123</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>69001</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>10500</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>69123</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>69001</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>790</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>15000</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>30300</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>1200</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>3100</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>670</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improve(Imports de masse): Mise à jour des fichiers templates (#4845)
</commit_message>
<xml_diff>
--- a/web/static/documents/fichier_exemple_ma_cantine.xlsx
+++ b/web/static/documents/fichier_exemple_ma_cantine.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="fichier_exemple_ma_cantine" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="fichier_exemple_ma_cantine" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,73 +22,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
-    <t xml:space="preserve">SIRET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom de la cantine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code postal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIRET cuisine centrale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repas par jour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repas par an</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secteurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode de production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode de gestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secteur économique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestionnaires addtionnels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Année du diagnostic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environnement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autre EGAlim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailes total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailles EGAlim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viandes vollailles provenance France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produits aquatiques total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produits aquatiques EGAlim</t>
+    <t xml:space="preserve">siret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_insee_commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_postal_commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_livreur_repas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_gestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">année_bilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_totale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_siqo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_environnemental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_autres_egalim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes_egalim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_viandes_france</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_poissons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur_poissons_egalim</t>
   </si>
   <si>
     <t xml:space="preserve">000 000 000 00000</t>
@@ -196,12 +196,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,253 +221,359 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="36.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="24.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="32.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="24.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>69123</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>69001</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>10500</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>69123</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>69001</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>790</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>15000</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>30300</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>1200</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>3100</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>670</v>
       </c>
     </row>

</xml_diff>